<commit_message>
Added other results for analysis
</commit_message>
<xml_diff>
--- a/initial_result.xlsx
+++ b/initial_result.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40182166\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40182166\Documents\GitHub\CPS-Coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Sample per pixel: </t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>400 x 400</t>
+  </si>
+  <si>
+    <t>1024x1024</t>
   </si>
 </sst>
 </file>
@@ -703,8 +706,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.6936943024001617E-5"/>
-                  <c:y val="-2.1116138763197588E-2"/>
+                  <c:x val="-5.8013907338822661E-2"/>
+                  <c:y val="-4.2232277526395287E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -720,6 +723,54 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-52BE-4564-AC4A-053F8C24221B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.1317281295026284E-2"/>
+                  <c:y val="9.0497737556561094E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-61CC-431B-B395-13B302501094}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-3.6199095022624493E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-61CC-431B-B395-13B302501094}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -768,6 +819,30 @@
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-52BE-4564-AC4A-053F8C24221B}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.5658640647513149E-3"/>
+                  <c:y val="4.2232277526395176E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-61CC-431B-B395-13B302501094}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -890,6 +965,206 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>initial_result!$D$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024x1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.1117634859734335E-2"/>
+                  <c:y val="-3.7684825595895532E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-61CC-431B-B395-13B302501094}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.1035425763371063E-2"/>
+                  <c:y val="1.9630408189926486E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-61CC-431B-B395-13B302501094}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>initial_result!$B$9:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>13592</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51321</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>201578</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>827554</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3218981</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>initial_result!$A$9:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-61CC-431B-B395-13B302501094}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
@@ -906,7 +1181,7 @@
         <c:axId val="443786112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2000000"/>
+          <c:max val="3300000"/>
           <c:min val="2000"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1021,7 +1296,7 @@
         <c:crossAx val="443786440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="200000"/>
+        <c:majorUnit val="300000"/>
         <c:minorUnit val="50000"/>
       </c:valAx>
       <c:valAx>
@@ -2085,16 +2360,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2154,6 +2430,49 @@
       </c>
       <c r="B7">
         <v>1946102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>13592</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>51321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>64</v>
+      </c>
+      <c r="B11">
+        <v>201578</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>256</v>
+      </c>
+      <c r="B12">
+        <v>827554</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1024</v>
+      </c>
+      <c r="B13">
+        <v>3218981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Analysis on different hardware and with more objects in scene
</commit_message>
<xml_diff>
--- a/initial_result.xlsx
+++ b/initial_result.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40182166\Documents\GitHub\CPS-Coursework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\Università\Year 4\Concurrent of Parrallel Systems\Coursework1\CPS-Coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial_result" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">initial_result!$A$1:$B$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">initial_result!$A$2:$B$7</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t xml:space="preserve">Sample per pixel: </t>
   </si>
@@ -35,11 +35,23 @@
   <si>
     <t>1024x1024</t>
   </si>
+  <si>
+    <t>Dimension:</t>
+  </si>
+  <si>
+    <t>Games Lab</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time taken(s): </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -517,52 +529,55 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Calcolo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cella collegata" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Cella da controllare" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Colore 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Colore 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Colore 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Colore 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Colore 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Colore 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Neutrale" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Testo avviso" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Testo descrittivo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titolo" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titolo 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titolo 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titolo 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titolo 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Totale" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -580,7 +595,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -617,7 +632,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -643,7 +657,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -668,7 +682,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>initial_result!$D$1</c:f>
+              <c:f>initial_result!$D$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -718,9 +732,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-52BE-4564-AC4A-053F8C24221B}"/>
                 </c:ext>
@@ -742,9 +754,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-61CC-431B-B395-13B302501094}"/>
                 </c:ext>
@@ -766,9 +776,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-61CC-431B-B395-13B302501094}"/>
                 </c:ext>
@@ -790,9 +798,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-52BE-4564-AC4A-053F8C24221B}"/>
                 </c:ext>
@@ -814,9 +820,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-52BE-4564-AC4A-053F8C24221B}"/>
                 </c:ext>
@@ -838,9 +842,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-61CC-431B-B395-13B302501094}"/>
                 </c:ext>
@@ -872,7 +874,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="r"/>
@@ -885,7 +887,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -906,34 +907,34 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>initial_result!$B$2:$B$7</c:f>
+              <c:f>initial_result!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2364</c:v>
+                  <c:v>2.3639999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9142</c:v>
+                  <c:v>9.1419999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30516</c:v>
+                  <c:v>30.515999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>121480</c:v>
+                  <c:v>121.48</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>484962</c:v>
+                  <c:v>484.96199999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1946102</c:v>
+                  <c:v>1946.1020000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>initial_result!$A$2:$A$7</c:f>
+              <c:f>initial_result!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -970,7 +971,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>initial_result!$D$9</c:f>
+              <c:f>initial_result!$D$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1020,9 +1021,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-61CC-431B-B395-13B302501094}"/>
                 </c:ext>
@@ -1044,9 +1043,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-61CC-431B-B395-13B302501094}"/>
                 </c:ext>
@@ -1078,7 +1075,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="it-IT"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1091,7 +1088,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1112,31 +1108,31 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>initial_result!$B$9:$B$13</c:f>
+              <c:f>initial_result!$B$10:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>13592</c:v>
+                  <c:v>13.592000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>51321</c:v>
+                  <c:v>51.320999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>201578</c:v>
+                  <c:v>201.578</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>827554</c:v>
+                  <c:v>827.55399999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3218981</c:v>
+                  <c:v>3218.9810000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>initial_result!$A$9:$A$13</c:f>
+              <c:f>initial_result!$A$10:$A$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1181,8 +1177,8 @@
         <c:axId val="443786112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="3300000"/>
-          <c:min val="2000"/>
+          <c:max val="3500"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1221,12 +1217,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Time Taken(ms)</a:t>
+                  <a:t>Time Taken(s)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1252,7 +1247,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="it-IT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1290,14 +1285,12 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="443786440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="300000"/>
-        <c:minorUnit val="50000"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="443786440"/>
@@ -1354,7 +1347,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1380,7 +1372,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="it-IT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1418,7 +1410,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="443786112"/>
@@ -1436,7 +1428,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1465,7 +1456,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="it-IT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1495,7 +1486,934 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Algorithm performance (Home)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.8386379008679164E-2"/>
+          <c:y val="0.11188536953242835"/>
+          <c:w val="0.90050823483537168"/>
+          <c:h val="0.68516312157812853"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>initial_result!$D$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>400 x 400</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.1145635468325285E-2"/>
+                  <c:y val="-7.1809346813014832E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-8B68-4B7F-B893-57F96A8D8205}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.1317281295026298E-3"/>
+                  <c:y val="-7.3765856907638094E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-8B68-4B7F-B893-57F96A8D8205}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.3951843885078899E-3"/>
+                  <c:y val="-3.619904654775296E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-8B68-4B7F-B893-57F96A8D8205}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="8.9335561485727761E-3"/>
+                  <c:y val="1.5082956259426848E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-8B68-4B7F-B893-57F96A8D8205}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.9009173004306251E-3"/>
+                  <c:y val="3.6022515819062934E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-8B68-4B7F-B893-57F96A8D8205}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.5658640647513149E-3"/>
+                  <c:y val="4.2232277526395176E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-8B68-4B7F-B893-57F96A8D8205}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>initial_result!$B$30:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4.6859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.411000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>242.78100000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>966.34400000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3850.1729999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>initial_result!$A$30:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-8B68-4B7F-B893-57F96A8D8205}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>initial_result!$D$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1024x1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.1117634859734335E-2"/>
+                  <c:y val="-3.7684825595895532E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000007-8B68-4B7F-B893-57F96A8D8205}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.8150290399970985E-2"/>
+                  <c:y val="-1.0329842310084018E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000A-8B68-4B7F-B893-57F96A8D8205}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.1035425763371063E-2"/>
+                  <c:y val="1.9630408189926486E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000008-8B68-4B7F-B893-57F96A8D8205}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>initial_result!$B$37:$B$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>26.279</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.918999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>401.762</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1569.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6249.5950000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>initial_result!$A$37:$A$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-8B68-4B7F-B893-57F96A8D8205}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="443786112"/>
+        <c:axId val="443786440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="443786112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="6500"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time Taken(s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="443786440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="443786440"/>
+        <c:scaling>
+          <c:logBase val="4"/>
+          <c:orientation val="minMax"/>
+          <c:max val="4096"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Sample per</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> pixel</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="443786112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1546,6 +2464,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2062,24 +3020,546 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>60007</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>245745</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2089,6 +3569,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>185738</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{395EE899-F5B4-4578-AA8B-FEE530D71D51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2359,124 +3877,275 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <f>2364/1000</f>
+        <v>2.3639999999999999</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <f>9142/1000</f>
+        <v>9.1419999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>64</v>
+      </c>
+      <c r="B5">
+        <f>30516/1000</f>
+        <v>30.515999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>256</v>
+      </c>
+      <c r="B6">
+        <f>121480/1000</f>
+        <v>121.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1024</v>
+      </c>
+      <c r="B7">
+        <f>484962/1000</f>
+        <v>484.96199999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4096</v>
+      </c>
+      <c r="B8">
+        <f>1946102/1000</f>
+        <v>1946.1020000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <f>13592/1000</f>
+        <v>13.592000000000001</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <f>51321/1000</f>
+        <v>51.320999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>64</v>
+      </c>
+      <c r="B12">
+        <f>201578/1000</f>
+        <v>201.578</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>256</v>
+      </c>
+      <c r="B13">
+        <f>827554/1000</f>
+        <v>827.55399999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1024</v>
+      </c>
+      <c r="B14">
+        <f>3218981/1000</f>
+        <v>3218.9810000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <f>4686/1000</f>
+        <v>4.6859999999999999</v>
+      </c>
+      <c r="D30" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <f>15590/1000</f>
+        <v>15.59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>64</v>
+      </c>
+      <c r="B32">
+        <f>60411/1000</f>
+        <v>60.411000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>256</v>
+      </c>
+      <c r="B33">
+        <f>242781/1000</f>
+        <v>242.78100000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>1024</v>
+      </c>
+      <c r="B34">
+        <f>966344/1000</f>
+        <v>966.34400000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>4096</v>
+      </c>
+      <c r="B35">
+        <f>3850173/1000</f>
+        <v>3850.1729999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>2364</v>
+      <c r="B37">
+        <f>26279/1000</f>
+        <v>26.279</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
         <v>16</v>
       </c>
-      <c r="B3">
-        <v>9142</v>
+      <c r="B38">
+        <f>99919/1000</f>
+        <v>99.918999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
         <v>64</v>
       </c>
-      <c r="B4">
-        <v>30516</v>
+      <c r="B39">
+        <f>401762/1000</f>
+        <v>401.762</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
         <v>256</v>
       </c>
-      <c r="B5">
-        <v>121480</v>
+      <c r="B40">
+        <f>1569080/1000</f>
+        <v>1569.08</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>1024</v>
       </c>
-      <c r="B6">
-        <v>484962</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4096</v>
-      </c>
-      <c r="B7">
-        <v>1946102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>13592</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>51321</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>64</v>
-      </c>
-      <c r="B11">
-        <v>201578</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>256</v>
-      </c>
-      <c r="B12">
-        <v>827554</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1024</v>
-      </c>
-      <c r="B13">
-        <v>3218981</v>
+      <c r="B41">
+        <f>6249595/1000</f>
+        <v>6249.5950000000003</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A28:D28"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Threads (with mutex and lock guards) and futures (*) implemented
*futures need to be revised as the implementation is probably not correct
</commit_message>
<xml_diff>
--- a/initial_result.xlsx
+++ b/initial_result.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
   <si>
     <t xml:space="preserve">Sample per pixel: </t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t xml:space="preserve">Time taken(s): </t>
+  </si>
+  <si>
+    <t>Home - changing spheres number</t>
+  </si>
+  <si>
+    <t>9 Spheres</t>
+  </si>
+  <si>
+    <t>14 Spheres</t>
+  </si>
+  <si>
+    <t>20 Spheres</t>
   </si>
 </sst>
 </file>
@@ -2424,6 +2436,1224 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Algorithm performance based on number of spheres of a 400x400 image</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="5.8386379008679164E-2"/>
+          <c:y val="0.11188536953242835"/>
+          <c:w val="0.90050823483537168"/>
+          <c:h val="0.68516312157812853"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>initial_result!$E$58</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>9 Spheres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.1145635468325285E-2"/>
+                  <c:y val="-7.1809346813014832E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.7936970395798648E-2"/>
+                  <c:y val="-7.3765856907638094E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.1673514136793393E-2"/>
+                  <c:y val="-9.2395438147871323E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.839859205394269E-2"/>
+                  <c:y val="-7.9563657027343637E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.4574431437224132E-2"/>
+                  <c:y val="-6.4539448096938221E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.5658640647513149E-3"/>
+                  <c:y val="4.2232277526395176E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>initial_result!$B$59:$B$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.6859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.59</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60.411000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>242.78100000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>966.34400000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>initial_result!$A$59:$A$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-1A05-43CD-A7D6-63E039099BD0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>initial_result!$E$65</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>14 Spheres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.4217299330121036E-2"/>
+                  <c:y val="-2.8076071236437062E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000010-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.0688769625189885E-2"/>
+                  <c:y val="7.4163866162692393E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000F-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.3599216229552085E-3"/>
+                  <c:y val="-0.13751114961561486"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000E-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.2238874905709094E-3"/>
+                  <c:y val="-9.6103282120790862E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000D-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.07222529504208E-2"/>
+                  <c:y val="-9.9060986941849685E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{0000000C-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>initial_result!$B$65:$B$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.952</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.126999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69.436999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>274.37799999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1088.4590000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>initial_result!$A$65:$A$69</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-1A05-43CD-A7D6-63E039099BD0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>initial_result!$E$71</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20 Spheres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.1411664337977653E-2"/>
+                  <c:y val="-8.1314758015496508E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000017-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.2080542171034591E-2"/>
+                  <c:y val="-5.1737709804908036E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000016-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="3.3136374122388929E-2"/>
+                  <c:y val="-1.032984231008391E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000015-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.4918191196249213E-3"/>
+                  <c:y val="4.290884446897554E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000014-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.4727303987499279E-2"/>
+                  <c:y val="-6.06108242680845E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000013-1A05-43CD-A7D6-63E039099BD0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>initial_result!$B$71:$B$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.4820000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.167000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.358999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>304.05500000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1236.1279999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>initial_result!$A$71:$A$75</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-1A05-43CD-A7D6-63E039099BD0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="443786112"/>
+        <c:axId val="443786440"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="443786112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1250"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time Taken(s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="443786440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="100"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="443786440"/>
+        <c:scaling>
+          <c:logBase val="4"/>
+          <c:orientation val="minMax"/>
+          <c:max val="4096"/>
+          <c:min val="4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Sample per pixel</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="it-IT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="443786112"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2504,6 +3734,43 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3536,20 +4803,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>60007</xdr:colOff>
+      <xdr:colOff>6667</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>49530</xdr:rowOff>
+      <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>245745</xdr:colOff>
+      <xdr:colOff>192405</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>99060</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3585,7 +5368,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>185738</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3607,6 +5390,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF3891A0-BF45-4C1A-96D9-CE506C52A58C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3878,10 +5699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="U64" sqref="U64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3889,6 +5710,7 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -4139,10 +5961,183 @@
         <v>6249.5950000000003</v>
       </c>
     </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>4</v>
+      </c>
+      <c r="B59">
+        <f>4686/1000</f>
+        <v>4.6859999999999999</v>
+      </c>
+      <c r="D59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>16</v>
+      </c>
+      <c r="B60">
+        <f>15590/1000</f>
+        <v>15.59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>64</v>
+      </c>
+      <c r="B61">
+        <f>60411/1000</f>
+        <v>60.411000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>256</v>
+      </c>
+      <c r="B62">
+        <f>242781/1000</f>
+        <v>242.78100000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>1024</v>
+      </c>
+      <c r="B63">
+        <f>966344/1000</f>
+        <v>966.34400000000005</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>4</v>
+      </c>
+      <c r="B65">
+        <f>4952/1000</f>
+        <v>4.952</v>
+      </c>
+      <c r="D65" t="s">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>16</v>
+      </c>
+      <c r="B66">
+        <f>18127/1000</f>
+        <v>18.126999999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>64</v>
+      </c>
+      <c r="B67">
+        <f>69437/1000</f>
+        <v>69.436999999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>256</v>
+      </c>
+      <c r="B68">
+        <f>274378/1000</f>
+        <v>274.37799999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>1024</v>
+      </c>
+      <c r="B69">
+        <f>1088459/1000</f>
+        <v>1088.4590000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>4</v>
+      </c>
+      <c r="B71">
+        <f>5482/1000</f>
+        <v>5.4820000000000002</v>
+      </c>
+      <c r="D71" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>16</v>
+      </c>
+      <c r="B72">
+        <f>20167/1000</f>
+        <v>20.167000000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>64</v>
+      </c>
+      <c r="B73">
+        <f>77359/1000</f>
+        <v>77.358999999999995</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>256</v>
+      </c>
+      <c r="B74">
+        <f>304055/1000</f>
+        <v>304.05500000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>1024</v>
+      </c>
+      <c r="B75">
+        <f>1236128/1000</f>
+        <v>1236.1279999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A57:D57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>